<commit_message>
use multiprocess and main page optimize
</commit_message>
<xml_diff>
--- a/res/10000078.xlsx
+++ b/res/10000078.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="296">
-  <si>
-    <t>알하이탐</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="300">
+  <si>
+    <t>艾尔海森</t>
   </si>
   <si>
     <t>Rarity</t>
@@ -49,22 +49,22 @@
     <t>Promote Costs</t>
   </si>
   <si>
-    <t>자라나는 비취 가루 x1, 모래 번데기 x3, 빛바랜 붉은 비단 x3</t>
-  </si>
-  <si>
-    <t>자라나는 비취 조각 x3, 창색의 날개꽃 x2, 모래 번데기 x10, 빛바랜 붉은 비단 x15</t>
-  </si>
-  <si>
-    <t>자라나는 비취 조각 x6, 창색의 날개꽃 x4, 모래 번데기 x20, 장식된 붉은 비단 x12</t>
-  </si>
-  <si>
-    <t>자라나는 비취 덩이 x3, 창색의 날개꽃 x8, 모래 번데기 x30, 장식된 붉은 비단 x18</t>
-  </si>
-  <si>
-    <t>자라나는 비취 덩이 x6, 창색의 날개꽃 x12, 모래 번데기 x45, 금자수 붉은 비단 x12</t>
-  </si>
-  <si>
-    <t>자라나는 비취 x6, 창색의 날개꽃 x20, 모래 번데기 x60, 금자수 붉은 비단 x24</t>
+    <t>生长碧翡碎屑 x1, 沙脂蛹 x3, 褪色红绸 x3</t>
+  </si>
+  <si>
+    <t>生长碧翡断片 x3, 苍砾蕊羽 x2, 沙脂蛹 x10, 褪色红绸 x15</t>
+  </si>
+  <si>
+    <t>生长碧翡断片 x6, 苍砾蕊羽 x4, 沙脂蛹 x20, 镶边红绸 x12</t>
+  </si>
+  <si>
+    <t>生长碧翡块 x3, 苍砾蕊羽 x8, 沙脂蛹 x30, 镶边红绸 x18</t>
+  </si>
+  <si>
+    <t>生长碧翡块 x6, 苍砾蕊羽 x12, 沙脂蛹 x45, 织金红绸 x12</t>
+  </si>
+  <si>
+    <t>生长碧翡 x6, 苍砾蕊羽 x20, 沙脂蛹 x60, 织金红绸 x24</t>
   </si>
   <si>
     <t>Skill Upgrade Costs</t>
@@ -73,55 +73,55 @@
     <t>Lv.2</t>
   </si>
   <si>
-    <t>「창의」의 가르침 x3, 빛바랜 붉은 비단 x6</t>
+    <t>「巧思」的教导 x3, 褪色红绸 x6</t>
   </si>
   <si>
     <t>Lv.3</t>
   </si>
   <si>
-    <t>「창의」의 인도 x2, 장식된 붉은 비단 x3</t>
+    <t>「巧思」的指引 x2, 镶边红绸 x3</t>
   </si>
   <si>
     <t>Lv.4</t>
   </si>
   <si>
-    <t>「창의」의 인도 x4, 장식된 붉은 비단 x4</t>
+    <t>「巧思」的指引 x4, 镶边红绸 x4</t>
   </si>
   <si>
     <t>Lv.5</t>
   </si>
   <si>
-    <t>「창의」의 인도 x6, 장식된 붉은 비단 x6</t>
+    <t>「巧思」的指引 x6, 镶边红绸 x6</t>
   </si>
   <si>
     <t>Lv.6</t>
   </si>
   <si>
-    <t>「창의」의 인도 x9, 장식된 붉은 비단 x9</t>
+    <t>「巧思」的指引 x9, 镶边红绸 x9</t>
   </si>
   <si>
     <t>Lv.7</t>
   </si>
   <si>
-    <t>「창의」의 철학 x4, 금자수 붉은 비단 x4, 무념의 거울 x1</t>
+    <t>「巧思」的哲学 x4, 织金红绸 x4, 无心的渊镜 x1</t>
   </si>
   <si>
     <t>Lv.8</t>
   </si>
   <si>
-    <t>「창의」의 철학 x6, 금자수 붉은 비단 x6, 무념의 거울 x1</t>
+    <t>「巧思」的哲学 x6, 织金红绸 x6, 无心的渊镜 x1</t>
   </si>
   <si>
     <t>Lv.9</t>
   </si>
   <si>
-    <t>「창의」의 철학 x12, 금자수 붉은 비단 x9, 무념의 거울 x2</t>
+    <t>「巧思」的哲学 x12, 织金红绸 x9, 无心的渊镜 x2</t>
   </si>
   <si>
     <t>Lv.10</t>
   </si>
   <si>
-    <t>「창의」의 철학 x16, 금자수 붉은 비단 x12, 무념의 거울 x2, 지식의 왕관 x1</t>
+    <t>「巧思」的哲学 x16, 织金红绸 x12, 无心的渊镜 x2, 智识之冕 x1</t>
   </si>
   <si>
     <t>Constellations</t>
@@ -130,55 +130,56 @@
     <t>Real Value</t>
   </si>
   <si>
-    <t>직관</t>
-  </si>
-  <si>
-    <t>광막 공격이 적에게 명중하면 보편성·이데아 모사의 재사용 대기 시간이 1초 감소한다. 해당 효과는 1초마다 최대 1회 발동된다</t>
+    <t>直观</t>
+  </si>
+  <si>
+    <t>光幕攻击命中敌人时，将使共相·理式摹写的冷却时间减少1秒。该效果每1秒至多触发一次。</t>
   </si>
   <si>
     <t>[1.0, 1.0]</t>
   </si>
   <si>
-    <t>논증</t>
-  </si>
-  <si>
-    <t>알하이탐이 빛조각을 생성했을 때, 생성된 빛조각 1개당 원소 마스터리가 40pt 증가한다, 지속 시간: 8초. 해당 효과는 최대 4스택까지 중첩되고, 각 스택의 지속 시간은 독립적으로 계산된다. 빛조각이 최대 수량에 도달해도 해당 효과는 발동된다</t>
+    <t>辩章</t>
+  </si>
+  <si>
+    <t>艾尔海森产生琢光镜时，每1枚产生的琢光镜将使元素精通提升40点，持续8秒。该效果最多叠加4层，每层独立计算持续时间。琢光镜数量达到上限时依然能触发该效果。</t>
   </si>
   <si>
     <t>[40.0, 8.0, 4.0]</t>
   </si>
   <si>
-    <t>반례</t>
-  </si>
-  <si>
-    <t>보편성·정밀 모사의 스킬 레벨+3. 최대 Lv.15까지 상승</t>
+    <t>遮诠</t>
+  </si>
+  <si>
+    <t>共相·理式摹写的技能等级提高3级。至多提升至15级。</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>해명</t>
-  </si>
-  <si>
-    <t>특정성·현상의 족쇄 발동 시 방금 소모 또는 생성된 집광 렌즈의 수에 따라 다음 효과가 발동된다.
-·소모된 집광 렌즈 1개당 자신과 다른 파티원의 원소 마스터리가 30 증가한다. 지속 시간: 15초
-·생성된 집광 렌즈 1개당 알하이탐이 10%의 풀 원소 피해 보너스를 획득한다. 지속 시간: 15초</t>
+    <t>义贯</t>
+  </si>
+  <si>
+    <t>施放殊境·显象缚结时，会依据通过本次施放消耗与产生的琢光镜数量，产生如下效果：
+·每消耗1枚琢光镜，使队伍中的其他角色元素精通提升30点，持续15秒；
+·每产生1枚琢光镜，使艾尔海森获得10%草元素伤害加成，持续15秒。
+上述效果的持续期间内重复施放殊境·显象缚结时，将先移除原有的效果。</t>
   </si>
   <si>
     <t>[30.0, 15.0, 0.10000000149011612, 15.0]</t>
   </si>
   <si>
-    <t>총명함</t>
-  </si>
-  <si>
-    <t>특정성·현상의 족쇄의 스킬 레벨+3. 최대 Lv.15까지 상승</t>
-  </si>
-  <si>
-    <t>정리</t>
-  </si>
-  <si>
-    <t>알하이탐이 집광 렌즈를 생성했을 때 렌즈의 수가 한도에 도달했을 경우, 한도를 초과한 렌즈 1개당 알하이탐의 치명타 확률이 10%, 치명타 피해가 70% 증가한다. 지속 시간: 6초
-지속 시간 동안 해당 효과가 다시 발동할 경우 지속 시간이 6초 증가한다</t>
+    <t>智度</t>
+  </si>
+  <si>
+    <t>殊境·显象缚结的技能等级提高3级。至多提升至15级。</t>
+  </si>
+  <si>
+    <t>正理</t>
+  </si>
+  <si>
+    <t>艾尔海森产生琢光镜时，若琢光镜数量已达到上限，艾尔海森的暴击率提升10%，暴击伤害提升70%，持续6秒。
+该效果在持续期间重复触发时，剩余持续时间将增加6秒。</t>
   </si>
   <si>
     <t>[0.10000000149011612, 0.699999988079071, 6.0]</t>
@@ -187,40 +188,40 @@
     <t>Passives</t>
   </si>
   <si>
-    <t>4단 인과 논증</t>
-  </si>
-  <si>
-    <t>알하이탐의 강공격 및 낙하 공격이 적에게 적중하면 집광 렌즈 1개를 생성한다. 해당 효과는 12초마다 최대 1회 발동한다</t>
+    <t>四因订顽</t>
+  </si>
+  <si>
+    <t>艾尔海森的重击或下落攻击命中敌人时，将产生一枚琢光镜。该效果每12秒至多触发一次。</t>
   </si>
   <si>
     <t>[12.0]</t>
   </si>
   <si>
-    <t>밝혀진 비밀</t>
-  </si>
-  <si>
-    <t>알하이탐의 원소 마스터리 1pt당 광선 피해와 특정성·현상의 족쇄가 가하는 피해가 0.1% 증가한다.
-해당 방식으로 광선과 특정성·현상의 족쇄의 피해는 최대 100%까지 증가한다</t>
+    <t>谜林道破</t>
+  </si>
+  <si>
+    <t>艾尔海森的每点元素精通，都会使光幕伤害与殊境·显象缚结造成的伤害提升0.12%。
+通过这种方式，至多使光幕伤害与殊境·显象缚结造成的伤害提升100%。</t>
   </si>
   <si>
     <t>[0.0012000000569969416, 1.0]</t>
   </si>
   <si>
-    <t>라이프 특성</t>
-  </si>
-  <si>
-    <t>무기 돌파 소재를 합성 시 10%의 확률로 생산량의 2배를 획득한다</t>
-  </si>
-  <si>
-    <t>일반 공격·인명의 검</t>
-  </si>
-  <si>
-    <t>일반 공격
-검으로 최대 5번 공격한다.
-강공격
-일정 스태미나를 소모해 순간적으로 전방을 향해 검을 2번 휘두른다.
-낙하 공격
-공중에서 땅을 내려찍어 경로상의 적을 공격하고, 착지 시 범위 피해를 준다</t>
+    <t>超定归约律</t>
+  </si>
+  <si>
+    <t>合成武器突破素材时，有10%概率获得2倍产出。</t>
+  </si>
+  <si>
+    <t>普通攻击·溯因反绎法</t>
+  </si>
+  <si>
+    <t>普通攻击
+进行至多五段的连续剑击。
+重击
+消耗一定体力，瞬间向前方挥出两剑。
+下落攻击
+从空中下坠冲击地面，攻击下落路径上的敌人，并在落地时造成范围伤害。</t>
   </si>
   <si>
     <t>Modifier</t>
@@ -244,7 +245,7 @@
     <t>Lv.15</t>
   </si>
   <si>
-    <t>1단 공격 피해</t>
+    <t>一段伤害</t>
   </si>
   <si>
     <t>56.0%</t>
@@ -292,7 +293,7 @@
     <t>149.9%</t>
   </si>
   <si>
-    <t>2단 공격 피해</t>
+    <t>二段伤害</t>
   </si>
   <si>
     <t>56.8%</t>
@@ -340,7 +341,7 @@
     <t>152.0%</t>
   </si>
   <si>
-    <t>3단 공격 피해</t>
+    <t>三段伤害</t>
   </si>
   <si>
     <t>37.2%+37.2%</t>
@@ -388,7 +389,7 @@
     <t>99.6%+99.6%</t>
   </si>
   <si>
-    <t>4단 공격 피해</t>
+    <t>四段伤害</t>
   </si>
   <si>
     <t>73.5%</t>
@@ -436,7 +437,7 @@
     <t>196.6%</t>
   </si>
   <si>
-    <t>5단 공격 피해</t>
+    <t>五段伤害</t>
   </si>
   <si>
     <t>96.5%</t>
@@ -481,7 +482,7 @@
     <t>258.2%</t>
   </si>
   <si>
-    <t>강공격 피해</t>
+    <t>重击伤害</t>
   </si>
   <si>
     <t>71.2%+71.2%</t>
@@ -529,13 +530,13 @@
     <t>190.4%+190.4%</t>
   </si>
   <si>
-    <t>강공격 스태미나 소모</t>
-  </si>
-  <si>
-    <t>20.0pt</t>
-  </si>
-  <si>
-    <t>낙하 기간 피해</t>
+    <t>重击体力消耗</t>
+  </si>
+  <si>
+    <t>20.0点</t>
+  </si>
+  <si>
+    <t>下坠期间伤害</t>
   </si>
   <si>
     <t>63.9%</t>
@@ -580,7 +581,7 @@
     <t>171.0%</t>
   </si>
   <si>
-    <t>저공/고공 추락 충격 피해</t>
+    <t>低空/高空坠地冲击伤害</t>
   </si>
   <si>
     <t>128%/160%</t>
@@ -628,303 +629,311 @@
     <t>342%/427%</t>
   </si>
   <si>
-    <t>보편성·정밀 모사</t>
-  </si>
-  <si>
-    <t>빠르게 돌진한 다음 주변의 적에게 풀 원소 피해를 주고 「집광 렌즈」를 생성한다.
-홀드 시 각기 다른 방식으로 발동한다.
-홀드
-조준 상태로 돌입해서 돌진할 방향을 결정한다.
-집광 렌즈
-스킬 발동 시 알하이탐이 집광 렌즈 1개를 생성한다. 만약 집광 렌즈가 하나도 없을 경우 1개를 추가로 생성한다. 집광 렌즈의 효과는 다음과 같다.
-·집광 렌즈를 보유하고 있을 경우 알하이탐의 일반 공격과 강공격, 낙하 공격으로 가하는 피해가 다른 원소 부여 효과로 대체될 수 없는 풀 원소 피해로 전환된다.
-·위 공격이 적에게 명중하면 집광 렌즈가 적에게 광선 공격을 가해서 집광 렌즈 개수에 비례하는 풀 원소 범위 피해를 준다.
-·집광 렌즈는 최대 3개까지 보유할 수 있다.
-·집광 렌즈는 시간이 지나면 사라지며, 알하이탐이 퇴장하면 전부 사라진다.
-&lt;i&gt;「진리는 불확실성 속에 존재하기 때문에 아무리 위대한 학자일지라도 오류를 피할 수 없다」&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>돌진 공격 피해</t>
-  </si>
-  <si>
-    <t>공격력의 196.0%+원소 마스터리의 392.0%</t>
-  </si>
-  <si>
-    <t>공격력의 210.7%+원소 마스터리의 421.4%</t>
-  </si>
-  <si>
-    <t>공격력의 225.4%+원소 마스터리의 450.8%</t>
-  </si>
-  <si>
-    <t>공격력의 245.0%+원소 마스터리의 490.0%</t>
-  </si>
-  <si>
-    <t>공격력의 259.7%+원소 마스터리의 519.4%</t>
-  </si>
-  <si>
-    <t>공격력의 274.4%+원소 마스터리의 548.8%</t>
-  </si>
-  <si>
-    <t>공격력의 294.0%+원소 마스터리의 588.0%</t>
-  </si>
-  <si>
-    <t>공격력의 313.6%+원소 마스터리의 627.2%</t>
-  </si>
-  <si>
-    <t>공격력의 333.2%+원소 마스터리의 666.4%</t>
-  </si>
-  <si>
-    <t>공격력의 352.8%+원소 마스터리의 705.6%</t>
-  </si>
-  <si>
-    <t>공격력의 372.4%+원소 마스터리의 744.8%</t>
-  </si>
-  <si>
-    <t>공격력의 392.0%+원소 마스터리의 784.0%</t>
-  </si>
-  <si>
-    <t>공격력의 416.5%+원소 마스터리의 833.0%</t>
-  </si>
-  <si>
-    <t>공격력의 441.0%+원소 마스터리의 882.0%</t>
-  </si>
-  <si>
-    <t>공격력의 465.5%+원소 마스터리의 931.0%</t>
-  </si>
-  <si>
-    <t>광선 공격 간격</t>
-  </si>
-  <si>
-    <t>1.6초</t>
-  </si>
-  <si>
-    <t>렌즈 1개 광선 공격 피해</t>
-  </si>
-  <si>
-    <t>공격력의 96.0%+원소 마스터리의 192.0%</t>
-  </si>
-  <si>
-    <t>공격력의 103.2%+원소 마스터리의 206.4%</t>
-  </si>
-  <si>
-    <t>공격력의 110.4%+원소 마스터리의 220.8%</t>
-  </si>
-  <si>
-    <t>공격력의 120.0%+원소 마스터리의 240.0%</t>
-  </si>
-  <si>
-    <t>공격력의 127.2%+원소 마스터리의 254.4%</t>
-  </si>
-  <si>
-    <t>공격력의 134.4%+원소 마스터리의 268.8%</t>
-  </si>
-  <si>
-    <t>공격력의 144.0%+원소 마스터리의 288.0%</t>
-  </si>
-  <si>
-    <t>공격력의 153.6%+원소 마스터리의 307.2%</t>
-  </si>
-  <si>
-    <t>공격력의 163.2%+원소 마스터리의 326.4%</t>
-  </si>
-  <si>
-    <t>공격력의 172.8%+원소 마스터리의 345.6%</t>
-  </si>
-  <si>
-    <t>공격력의 182.4%+원소 마스터리의 364.8%</t>
-  </si>
-  <si>
-    <t>공격력의 192.0%+원소 마스터리의 384.0%</t>
-  </si>
-  <si>
-    <t>공격력의 204.0%+원소 마스터리의 408.0%</t>
-  </si>
-  <si>
-    <t>공격력의 216.0%+원소 마스터리의 432.0%</t>
-  </si>
-  <si>
-    <t>공격력의 228.0%+원소 마스터리의 456.0%</t>
-  </si>
-  <si>
-    <t>렌즈 2개 광선 공격 피해</t>
-  </si>
-  <si>
-    <t>공격력의 64.0%+원소 마스터리의 128.0%</t>
-  </si>
-  <si>
-    <t>공격력의 68.8%+원소 마스터리의 137.6%</t>
-  </si>
-  <si>
-    <t>공격력의 73.6%+원소 마스터리의 147.2%</t>
-  </si>
-  <si>
-    <t>공격력의 80.0%+원소 마스터리의 160.0%</t>
-  </si>
-  <si>
-    <t>공격력의 84.8%+원소 마스터리의 169.6%</t>
-  </si>
-  <si>
-    <t>공격력의 89.6%+원소 마스터리의 179.2%</t>
-  </si>
-  <si>
-    <t>공격력의 102.4%+원소 마스터리의 204.8%</t>
-  </si>
-  <si>
-    <t>공격력의 108.8%+원소 마스터리의 217.6%</t>
-  </si>
-  <si>
-    <t>공격력의 115.2%+원소 마스터리의 230.4%</t>
-  </si>
-  <si>
-    <t>공격력의 121.6%+원소 마스터리의 243.2%</t>
-  </si>
-  <si>
-    <t>공격력의 128.0%+원소 마스터리의 256.0%</t>
-  </si>
-  <si>
-    <t>공격력의 136.0%+원소 마스터리의 272.0%</t>
-  </si>
-  <si>
-    <t>공격력의 152.0%+원소 마스터리의 304.0%</t>
-  </si>
-  <si>
-    <t>렌즈 3개 광선 공격 피해</t>
-  </si>
-  <si>
-    <t>공격력의 53.4%+원소 마스터리의 106.7%</t>
-  </si>
-  <si>
-    <t>공격력의 57.4%+원소 마스터리의 114.7%</t>
-  </si>
-  <si>
-    <t>공격력의 61.4%+원소 마스터리의 122.7%</t>
-  </si>
-  <si>
-    <t>공격력의 66.7%+원소 마스터리의 133.4%</t>
-  </si>
-  <si>
-    <t>공격력의 70.7%+원소 마스터리의 141.4%</t>
-  </si>
-  <si>
-    <t>공격력의 74.7%+원소 마스터리의 149.4%</t>
-  </si>
-  <si>
-    <t>공격력의 80.0%+원소 마스터리의 160.1%</t>
-  </si>
-  <si>
-    <t>공격력의 85.4%+원소 마스터리의 170.8%</t>
-  </si>
-  <si>
-    <t>공격력의 90.7%+원소 마스터리의 181.4%</t>
-  </si>
-  <si>
-    <t>공격력의 96.0%+원소 마스터리의 192.1%</t>
-  </si>
-  <si>
-    <t>공격력의 101.4%+원소 마스터리의 202.8%</t>
-  </si>
-  <si>
-    <t>공격력의 106.7%+원소 마스터리의 213.4%</t>
-  </si>
-  <si>
-    <t>공격력의 113.4%+원소 마스터리의 226.8%</t>
-  </si>
-  <si>
-    <t>공격력의 120.1%+원소 마스터리의 240.1%</t>
-  </si>
-  <si>
-    <t>공격력의 126.7%+원소 마스터리의 253.5%</t>
-  </si>
-  <si>
-    <t>집광 렌즈 소멸 간격</t>
-  </si>
-  <si>
-    <t>4.0초</t>
-  </si>
-  <si>
-    <t>재사용 대기시간</t>
-  </si>
-  <si>
-    <t>18.0초</t>
-  </si>
-  <si>
-    <t>특정성·현상의 족쇄</t>
-  </si>
-  <si>
-    <t>특수 렌즈를 소환해서 여러 번에 걸쳐 풀 원소 범위 피해를 준다.
-스킬 발동 시 집광 렌즈가 존재할 경우, 집광 렌즈를 모두 소모하는 대신 공격 횟수가 증가한다.
-발동 완료 2초 후 집광 렌즈가 생성된다. 이때 생성되는 집광 렌즈의 수는 해당 스킬 발동으로 인해 소모되었던 집광 렌즈의 수에 따라 결정된다.
-·집광 렌즈를 소모하지 않았을 경우 3개가 생성된다.
-·렌즈를 1개 소모했을 경우 2개가 생성된다.
-·렌즈를 2개 소모했을 경우 1개가 생성된다.
-·렌즈를 3개 소모했을 경우 렌즈가 생성되지 않는다.
-&lt;i&gt;「무릇 지혜를 추구하는 것을 목표로 삼은 학자라면 책의 글자 하나하나를 적을 대하듯이 해야 한다. 그래야만 편견에 휘말리는 것을 피할 수 있으니까」&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t>1회 피해</t>
-  </si>
-  <si>
-    <t>공격력의 130.7%+원소 마스터리의 261.4%</t>
-  </si>
-  <si>
-    <t>공격력의 139.8%+원소 마스터리의 279.7%</t>
-  </si>
-  <si>
-    <t>공격력의 161.1%+원소 마스터리의 322.2%</t>
-  </si>
-  <si>
-    <t>공격력의 170.2%+원소 마스터리의 340.5%</t>
-  </si>
-  <si>
-    <t>공격력의 194.6%+원소 마스터리의 389.1%</t>
-  </si>
-  <si>
-    <t>공격력의 206.7%+원소 마스터리의 413.4%</t>
-  </si>
-  <si>
-    <t>공격력의 218.9%+원소 마스터리의 437.8%</t>
-  </si>
-  <si>
-    <t>공격력의 231.0%+원소 마스터리의 462.1%</t>
-  </si>
-  <si>
-    <t>공격력의 243.2%+원소 마스터리의 486.4%</t>
-  </si>
-  <si>
-    <t>공격력의 258.4%+원소 마스터리의 516.8%</t>
-  </si>
-  <si>
-    <t>공격력의 273.6%+원소 마스터리의 547.2%</t>
-  </si>
-  <si>
-    <t>공격력의 288.8%+원소 마스터리의 577.6%</t>
-  </si>
-  <si>
-    <t>기본 공격 횟수</t>
-  </si>
-  <si>
-    <t>4회</t>
-  </si>
-  <si>
-    <t>렌즈 1개 공격 횟수</t>
-  </si>
-  <si>
-    <t>6회</t>
-  </si>
-  <si>
-    <t>렌즈 2개 공격 횟수</t>
-  </si>
-  <si>
-    <t>8회</t>
-  </si>
-  <si>
-    <t>렌즈 3개 공격 횟수</t>
-  </si>
-  <si>
-    <t>10회</t>
-  </si>
-  <si>
-    <t>원소 에너지</t>
+    <t>共相·理式摹写</t>
+  </si>
+  <si>
+    <t>迅速突进，在突进结束时对身边的敌人造成草元素伤害，并凝聚「琢光镜」。
+长按时将以不同的方式施放。
+长按
+进入瞄准状态，以调整突进的方向。
+琢光镜
+施放时，艾尔海森将产生1枚琢光镜；若此时未持有任何琢光镜，则额外产生1枚。琢光镜具有如下效果：
+·持有琢光镜时，艾尔海森的普通攻击、重击与下落攻击将转为无法被附魔覆盖的草元素伤害；
+·上述攻击命中敌人时，琢光镜将进行光幕攻击，造成基于琢光镜数量的草元素范围伤害；
+·至多持有3枚琢光镜；
+·琢光镜将随着时间流逝逐枚消失，并将在艾尔海森退场时全部消失。
+&lt;i&gt;「真理本就存在于不确定性当中，即便再伟大的学者也不能免于错谬。」&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>突进攻击伤害</t>
+  </si>
+  <si>
+    <t>196.0%攻击力+392.0%元素精通</t>
+  </si>
+  <si>
+    <t>210.7%攻击力+421.4%元素精通</t>
+  </si>
+  <si>
+    <t>225.4%攻击力+450.8%元素精通</t>
+  </si>
+  <si>
+    <t>245.0%攻击力+490.0%元素精通</t>
+  </si>
+  <si>
+    <t>259.7%攻击力+519.4%元素精通</t>
+  </si>
+  <si>
+    <t>274.4%攻击力+548.8%元素精通</t>
+  </si>
+  <si>
+    <t>294.0%攻击力+588.0%元素精通</t>
+  </si>
+  <si>
+    <t>313.6%攻击力+627.2%元素精通</t>
+  </si>
+  <si>
+    <t>333.2%攻击力+666.4%元素精通</t>
+  </si>
+  <si>
+    <t>352.8%攻击力+705.6%元素精通</t>
+  </si>
+  <si>
+    <t>372.4%攻击力+744.8%元素精通</t>
+  </si>
+  <si>
+    <t>392.0%攻击力+784.0%元素精通</t>
+  </si>
+  <si>
+    <t>416.5%攻击力+833.0%元素精通</t>
+  </si>
+  <si>
+    <t>441.0%攻击力+882.0%元素精通</t>
+  </si>
+  <si>
+    <t>465.5%攻击力+931.0%元素精通</t>
+  </si>
+  <si>
+    <t>光幕攻击间隔</t>
+  </si>
+  <si>
+    <t>1.6秒</t>
+  </si>
+  <si>
+    <t>1枚光幕攻击伤害</t>
+  </si>
+  <si>
+    <t>96.0%攻击力+192.0%元素精通</t>
+  </si>
+  <si>
+    <t>103.2%攻击力+206.4%元素精通</t>
+  </si>
+  <si>
+    <t>110.4%攻击力+220.8%元素精通</t>
+  </si>
+  <si>
+    <t>120.0%攻击力+240.0%元素精通</t>
+  </si>
+  <si>
+    <t>127.2%攻击力+254.4%元素精通</t>
+  </si>
+  <si>
+    <t>134.4%攻击力+268.8%元素精通</t>
+  </si>
+  <si>
+    <t>144.0%攻击力+288.0%元素精通</t>
+  </si>
+  <si>
+    <t>153.6%攻击力+307.2%元素精通</t>
+  </si>
+  <si>
+    <t>163.2%攻击力+326.4%元素精通</t>
+  </si>
+  <si>
+    <t>172.8%攻击力+345.6%元素精通</t>
+  </si>
+  <si>
+    <t>182.4%攻击力+364.8%元素精通</t>
+  </si>
+  <si>
+    <t>192.0%攻击力+384.0%元素精通</t>
+  </si>
+  <si>
+    <t>204.0%攻击力+408.0%元素精通</t>
+  </si>
+  <si>
+    <t>216.0%攻击力+432.0%元素精通</t>
+  </si>
+  <si>
+    <t>228.0%攻击力+456.0%元素精通</t>
+  </si>
+  <si>
+    <t>2枚光幕攻击伤害</t>
+  </si>
+  <si>
+    <t>(64.0%攻击力+128.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(68.8%攻击力+137.6%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(73.6%攻击力+147.2%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(80.0%攻击力+160.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(84.8%攻击力+169.6%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(89.6%攻击力+179.2%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(96.0%攻击力+192.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(102.4%攻击力+204.8%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(108.8%攻击力+217.6%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(115.2%攻击力+230.4%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(121.6%攻击力+243.2%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(128.0%攻击力+256.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(136.0%攻击力+272.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(144.0%攻击力+288.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>(152.0%攻击力+304.0%元素精通)*2</t>
+  </si>
+  <si>
+    <t>3枚光幕攻击伤害</t>
+  </si>
+  <si>
+    <t>(53.4%攻击力+106.7%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(57.4%攻击力+114.7%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(61.4%攻击力+122.7%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(66.7%攻击力+133.4%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(70.7%攻击力+141.4%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(74.7%攻击力+149.4%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(80.0%攻击力+160.1%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(85.4%攻击力+170.8%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(90.7%攻击力+181.4%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(96.0%攻击力+192.1%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(101.4%攻击力+202.8%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(106.7%攻击力+213.4%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(113.4%攻击力+226.8%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(120.1%攻击力+240.1%元素精通)*3</t>
+  </si>
+  <si>
+    <t>(126.7%攻击力+253.5%元素精通)*3</t>
+  </si>
+  <si>
+    <t>琢光镜消失间隔</t>
+  </si>
+  <si>
+    <t>4.0秒</t>
+  </si>
+  <si>
+    <t>冷却时间</t>
+  </si>
+  <si>
+    <t>18.0秒</t>
+  </si>
+  <si>
+    <t>殊境·显象缚结</t>
+  </si>
+  <si>
+    <t>创造殊相缚境，造成多次草元素范围伤害。
+施放时，若持有琢光镜，将消耗所有的琢光镜，增加造成伤害的次数。
+施放完成2秒后，若施放时消耗了0/1/2/3个琢光镜，则将为艾尔海森产生3/2/1/0个琢光镜。
+&lt;i&gt;「学者如果将追求智慧作为自己的目标，那么他就必须与他所读到的每一个字为敌，这样才有可能免于偏见。」&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>单次伤害</t>
+  </si>
+  <si>
+    <t>121.6%攻击力+243.2%元素精通</t>
+  </si>
+  <si>
+    <t>130.7%攻击力+261.4%元素精通</t>
+  </si>
+  <si>
+    <t>139.8%攻击力+279.7%元素精通</t>
+  </si>
+  <si>
+    <t>152.0%攻击力+304.0%元素精通</t>
+  </si>
+  <si>
+    <t>161.1%攻击力+322.2%元素精通</t>
+  </si>
+  <si>
+    <t>170.2%攻击力+340.5%元素精通</t>
+  </si>
+  <si>
+    <t>194.6%攻击力+389.1%元素精通</t>
+  </si>
+  <si>
+    <t>206.7%攻击力+413.4%元素精通</t>
+  </si>
+  <si>
+    <t>218.9%攻击力+437.8%元素精通</t>
+  </si>
+  <si>
+    <t>231.0%攻击力+462.1%元素精通</t>
+  </si>
+  <si>
+    <t>243.2%攻击力+486.4%元素精通</t>
+  </si>
+  <si>
+    <t>258.4%攻击力+516.8%元素精通</t>
+  </si>
+  <si>
+    <t>273.6%攻击力+547.2%元素精通</t>
+  </si>
+  <si>
+    <t>288.8%攻击力+577.6%元素精通</t>
+  </si>
+  <si>
+    <t>基本攻击次数</t>
+  </si>
+  <si>
+    <t>4次</t>
+  </si>
+  <si>
+    <t>1枚攻击次数</t>
+  </si>
+  <si>
+    <t>6次</t>
+  </si>
+  <si>
+    <t>2枚攻击次数</t>
+  </si>
+  <si>
+    <t>8次</t>
+  </si>
+  <si>
+    <t>3枚攻击次数</t>
+  </si>
+  <si>
+    <t>10次</t>
+  </si>
+  <si>
+    <t>元素能量</t>
   </si>
   <si>
     <t>70</t>
@@ -2643,186 +2652,186 @@
         <v>243</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:16">
       <c r="A58" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:16">
       <c r="A59" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2842,7 +2851,7 @@
     </row>
     <row r="63" spans="1:16" ht="200" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2912,352 +2921,352 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>232</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="66" spans="1:16">
       <c r="A66" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="P66" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="67" spans="1:16">
       <c r="A67" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:16">
       <c r="A68" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="P68" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:16">
       <c r="A69" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:16">
       <c r="A70" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>